<commit_message>
public email combine with AWS forward email successed . Trying to trigger ...
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects github\AWS-email-checking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CF23DC-0767-455B-BDF2-E82B7CC8D7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063514B5-34DB-42D1-ABA2-6C65274AEDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB17E63E-70F0-415D-9F71-47F3512487D7}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>Alice Manager</t>
   </si>
   <si>
-    <t>ecommerce_boss@company.com</t>
-  </si>
-  <si>
     <t>ecommerce, order, cart, payment</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>Bob AI Lead</t>
   </si>
   <si>
-    <t>ai_boss@company.com</t>
-  </si>
-  <si>
     <t>AI, ML, model, training, dataset</t>
   </si>
   <si>
@@ -85,17 +79,23 @@
     <t>Carol Engineer</t>
   </si>
   <si>
-    <t>se_boss@company.com</t>
-  </si>
-  <si>
     <t>chip, wafer, fabrication, semiconductor</t>
+  </si>
+  <si>
+    <t>yankin8913@gmail.com</t>
+  </si>
+  <si>
+    <t>dilaa9913@gmail.com</t>
+  </si>
+  <si>
+    <t>npcsstyles@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +110,17 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Google Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF444746"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,14 +144,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,10 +490,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
@@ -490,7 +501,7 @@
     <col min="4" max="4" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -512,15 +523,15 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="mailto:ecommerce_boss@company.com" xr:uid="{99F3EA44-35DC-4989-A32C-5740BA930591}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5242C5B6-CC09-4004-BEE6-FCA6B77949B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -531,16 +542,18 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="4" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -554,24 +567,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="mailto:ai_boss@company.com" xr:uid="{DA205E05-E1E3-4859-85C4-10D1BECA9BD6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -581,17 +591,18 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -605,24 +616,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="mailto:se_boss@company.com" xr:uid="{8040E855-3000-44B7-9477-D7423D95CEB0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>